<commit_message>
Pages Ready for Calculation.
</commit_message>
<xml_diff>
--- a/FillWeatherStat/5.xlsx
+++ b/FillWeatherStat/5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\shanzhashu\FillWeatherStat\Win32\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9F199D38-4616-47B2-8EB0-00F4BDB3C67F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDFAFB7C-A5EA-43F2-AD87-97D39966C27E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="-60" windowWidth="21720" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -385,9 +385,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -412,97 +409,100 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="31" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="20" fontId="7" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="31" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -845,8 +845,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:F7"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -861,299 +861,318 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="31.5" x14ac:dyDescent="0.15">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="27"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
+      <c r="A2" s="33"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
     </row>
     <row r="3" spans="1:6" ht="31.5" x14ac:dyDescent="0.15">
-      <c r="A3" s="6"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="42" t="s">
+      <c r="A3" s="5"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
     </row>
     <row r="4" spans="1:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="15"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="21"/>
     </row>
     <row r="5" spans="1:6" s="1" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="19">
+      <c r="B5" s="36">
         <v>0.54861111111111105</v>
       </c>
-      <c r="C5" s="20"/>
-      <c r="D5" s="12" t="s">
+      <c r="C5" s="37"/>
+      <c r="D5" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="19">
+      <c r="E5" s="36">
         <v>0.65972222222222221</v>
       </c>
-      <c r="F5" s="20"/>
+      <c r="F5" s="37"/>
     </row>
     <row r="6" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="15"/>
-      <c r="D6" s="13" t="s">
+      <c r="C6" s="21"/>
+      <c r="D6" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="14"/>
-      <c r="F6" s="15"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="21"/>
     </row>
     <row r="7" spans="1:6" ht="201" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="33"/>
-      <c r="B7" s="29" t="s">
+      <c r="A7" s="39"/>
+      <c r="B7" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="31"/>
-      <c r="D7" s="29" t="s">
+      <c r="C7" s="41"/>
+      <c r="D7" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="30"/>
-      <c r="F7" s="31"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="41"/>
     </row>
     <row r="8" spans="1:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="18"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="19"/>
     </row>
     <row r="9" spans="1:6" s="2" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="21">
+      <c r="A10" s="16">
         <v>950</v>
       </c>
       <c r="B10" s="3">
         <v>950</v>
       </c>
-      <c r="C10" s="39">
+      <c r="C10" s="22">
         <v>-0.04</v>
       </c>
-      <c r="D10" s="22">
+      <c r="D10" s="25">
         <f>AVERAGE(B10:B12)+C10</f>
         <v>949.96</v>
       </c>
-      <c r="E10" s="34">
+      <c r="E10" s="28">
         <v>950.1</v>
       </c>
-      <c r="F10" s="22">
+      <c r="F10" s="25">
         <f>E10-D10</f>
         <v>0.13999999999998636</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="21"/>
+      <c r="A11" s="16"/>
       <c r="B11" s="3">
         <v>950</v>
       </c>
-      <c r="C11" s="40"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="35"/>
-      <c r="F11" s="23"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="26"/>
     </row>
     <row r="12" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="21"/>
+      <c r="A12" s="16"/>
       <c r="B12" s="3">
         <v>950</v>
       </c>
-      <c r="C12" s="41"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="24"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="27"/>
     </row>
     <row r="13" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="21">
+      <c r="A13" s="16">
         <v>1000</v>
       </c>
       <c r="B13" s="3">
         <v>1000</v>
       </c>
-      <c r="C13" s="39">
+      <c r="C13" s="22">
         <v>-0.04</v>
       </c>
-      <c r="D13" s="22">
+      <c r="D13" s="25">
         <f>AVERAGE(B13:B15)+C13</f>
         <v>999.96</v>
       </c>
-      <c r="E13" s="34">
+      <c r="E13" s="28">
         <v>1000.1</v>
       </c>
-      <c r="F13" s="22">
+      <c r="F13" s="25">
         <f>E13-D13</f>
         <v>0.13999999999998636</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="21"/>
+      <c r="A14" s="16"/>
       <c r="B14" s="3">
         <v>1000</v>
       </c>
-      <c r="C14" s="40"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="35"/>
-      <c r="F14" s="23"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="26"/>
     </row>
     <row r="15" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="21"/>
+      <c r="A15" s="16"/>
       <c r="B15" s="3">
         <v>1000</v>
       </c>
-      <c r="C15" s="41"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="24"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="27"/>
     </row>
     <row r="16" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="21">
+      <c r="A16" s="16">
         <v>1050</v>
       </c>
       <c r="B16" s="3">
         <v>1050</v>
       </c>
-      <c r="C16" s="39">
+      <c r="C16" s="22">
         <v>-0.04</v>
       </c>
-      <c r="D16" s="22">
+      <c r="D16" s="25">
         <f>AVERAGE(B16:B18)+C16</f>
         <v>1049.96</v>
       </c>
-      <c r="E16" s="34">
+      <c r="E16" s="28">
         <v>1050</v>
       </c>
-      <c r="F16" s="22">
+      <c r="F16" s="25">
         <f>E16-D16</f>
         <v>3.999999999996362E-2</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="21"/>
+      <c r="A17" s="16"/>
       <c r="B17" s="3">
         <v>1050</v>
       </c>
-      <c r="C17" s="40"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="35"/>
-      <c r="F17" s="23"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="26"/>
     </row>
     <row r="18" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="21"/>
+      <c r="A18" s="16"/>
       <c r="B18" s="3">
         <v>1050</v>
       </c>
-      <c r="C18" s="41"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="24"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="27"/>
     </row>
     <row r="19" spans="1:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="21" t="s">
+      <c r="A19" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="21"/>
-      <c r="C19" s="16" t="s">
+      <c r="B19" s="16"/>
+      <c r="C19" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="19"/>
     </row>
     <row r="20" spans="1:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="13" t="s">
+      <c r="A20" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B20" s="15"/>
-      <c r="C20" s="16" t="s">
+      <c r="B20" s="21"/>
+      <c r="C20" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="19"/>
     </row>
     <row r="21" spans="1:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="13" t="s">
+      <c r="A21" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B21" s="15"/>
-      <c r="C21" s="16" t="s">
+      <c r="B21" s="21"/>
+      <c r="C21" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="18"/>
-    </row>
-    <row r="22" spans="1:6" s="9" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
-      <c r="A22" s="7" t="s">
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="19"/>
+    </row>
+    <row r="22" spans="1:6" s="8" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
+      <c r="A22" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="4"/>
-      <c r="C22" s="8" t="s">
+      <c r="B22" s="43"/>
+      <c r="C22" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D22" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E22" s="37">
+      <c r="E22" s="12">
         <v>45000</v>
       </c>
-      <c r="F22" s="38"/>
+      <c r="F22" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="34">
+  <mergeCells count="35">
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E16:E18"/>
+    <mergeCell ref="F16:F18"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="E10:E12"/>
+    <mergeCell ref="F10:F12"/>
     <mergeCell ref="E22:F22"/>
     <mergeCell ref="D3:F3"/>
     <mergeCell ref="A19:B19"/>
@@ -1170,27 +1189,9 @@
     <mergeCell ref="A16:A18"/>
     <mergeCell ref="C16:C18"/>
     <mergeCell ref="D16:D18"/>
-    <mergeCell ref="E16:E18"/>
-    <mergeCell ref="F16:F18"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="E10:E12"/>
-    <mergeCell ref="F10:F12"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:F7"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.47244094488188998" right="0.39370078740157499" top="0.74803149606299202" bottom="0.74803149606299202" header="0.31496062992126" footer="0.31496062992126"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>